<commit_message>
Modified the Timing Analysis spreadsheet
</commit_message>
<xml_diff>
--- a/FPGA_Developments/USB_3_FTDI/Documentation/Transfer Timing Analysis.xlsx
+++ b/FPGA_Developments/USB_3_FTDI/Documentation/Transfer Timing Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rfranca\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rfranca\Development\GitLab\simutemp\FPGA_Developments\USB_3_FTDI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2829B8AF-607C-4C68-83E5-7C6B5CEA5AF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37C4E55-4509-472A-ABA7-9BB2A4D737D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE54F853-42C2-447C-92F1-1D14CFBF6EF8}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EE54F853-42C2-447C-92F1-1D14CFBF6EF8}"/>
   </bookViews>
   <sheets>
     <sheet name="N-FEE" sheetId="1" r:id="rId1"/>
@@ -32,32 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
-  <si>
-    <t>Rows (px)</t>
-  </si>
-  <si>
-    <t>Pixel (bits)</t>
-  </si>
-  <si>
-    <t>Overscan (px)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>Total Pixels</t>
   </si>
   <si>
-    <t>Total Size (bits)</t>
-  </si>
-  <si>
-    <t>Total Size (Bytes)</t>
-  </si>
-  <si>
-    <t>E Columns (px)</t>
-  </si>
-  <si>
-    <t>F Columns (px)</t>
-  </si>
-  <si>
     <t>N-FEE caracteristics</t>
   </si>
   <si>
@@ -67,27 +46,6 @@
     <t>CCDs per camera</t>
   </si>
   <si>
-    <t>Readout Time (s)</t>
-  </si>
-  <si>
-    <t>Size per camera (bits)</t>
-  </si>
-  <si>
-    <t>Size per camera (Bytes)</t>
-  </si>
-  <si>
-    <t>Minimum data rate (bits/s)</t>
-  </si>
-  <si>
-    <t>Minimum data rate (Bytes/s)</t>
-  </si>
-  <si>
-    <t>Total Size (MBytes)</t>
-  </si>
-  <si>
-    <t>Minimum data rate (MBytes/s)</t>
-  </si>
-  <si>
     <t>F-FEE caracteristics</t>
   </si>
   <si>
@@ -100,9 +58,6 @@
     <t>Simulated cameras</t>
   </si>
   <si>
-    <t>Size per camera (MBytes)</t>
-  </si>
-  <si>
     <t>F-FEE CCD caracteristics</t>
   </si>
   <si>
@@ -130,9 +85,6 @@
     <t>Total Size [Bytes]</t>
   </si>
   <si>
-    <t>Total Size [Mbytes]</t>
-  </si>
-  <si>
     <t>Size per camera [bits]</t>
   </si>
   <si>
@@ -151,10 +103,13 @@
     <t>Minimum data rate [Bytes/s]</t>
   </si>
   <si>
-    <t>Minimum data rate [MBytes/s]</t>
-  </si>
-  <si>
     <t>Total Size [MBytes]</t>
+  </si>
+  <si>
+    <t>Minimum data rate [MiBytes/s]</t>
+  </si>
+  <si>
+    <t>Total Size [MiBytes]</t>
   </si>
 </sst>
 </file>
@@ -348,12 +303,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,12 +310,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -380,12 +323,6 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +332,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -713,235 +668,237 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442A95F5-89D9-4832-937A-D9521D552F4E}">
   <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="E2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="E2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
         <v>4510</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="19">
+      <c r="E3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5">
         <v>30</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="19">
+      <c r="E4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="13">
         <f>F3*C16</f>
         <v>10669363200</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
         <v>2295</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="19">
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="13">
         <f>F4/8</f>
         <v>1333670400</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5">
         <v>2295</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="20">
+      <c r="E6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="14">
         <f>F5/1024/1024</f>
         <v>1271.88720703125</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
         <f>(C3+C4)*(C5+C6)</f>
         <v>20838600</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="19">
+      <c r="E7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13">
         <f>F4/C19</f>
         <v>426774528</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5">
         <v>16</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="19">
+      <c r="E8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="13">
         <f>F7/8</f>
         <v>53346816</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5">
         <f>C7*C8</f>
         <v>333417600</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="22">
+      <c r="E9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="16">
         <f>F8/1024/1024</f>
         <v>50.87548828125</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="7">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
         <f>C9/8</f>
         <v>41677200</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="8">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6">
         <f>C10/1024/1024</f>
         <v>39.746475219726563</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="12">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="12">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8">
         <f>C15*C9</f>
         <v>1333670400</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="12">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="8">
         <f>C16/8</f>
         <v>166708800</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="13">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9">
         <f>C17/1024/1024</f>
         <v>158.98590087890625</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="12">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="12">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="8">
         <f>C16/C19</f>
         <v>53346816</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="12">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="8">
         <f>C20/8</f>
         <v>6668352</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="15">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="11">
         <f>C21/1024/1024</f>
         <v>6.35943603515625</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
   </sheetData>
@@ -959,239 +916,239 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDD0D2E-3209-4761-BD12-93CDA5EAFBEA}">
   <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="E2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="E2" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="6">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
         <f>4510/2</f>
         <v>2255</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="7">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5">
         <f>30/2</f>
         <v>15</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="19">
+      <c r="E4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="13">
         <f>F3*C16</f>
-        <v>1333670400</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>666835200</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="7">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
         <v>2295</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="19">
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="13">
         <f>F4/8</f>
-        <v>166708800</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+        <v>83354400</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="7">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5">
         <v>2295</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="20">
+      <c r="E6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="14">
         <f>F5/1024/1024</f>
-        <v>158.98590087890625</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+        <v>79.492950439453125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
         <f>(C3+C4)*(C5+C6)</f>
         <v>10419300</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="19">
+      <c r="E7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13">
         <f>F4/C19</f>
-        <v>533468160</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+        <v>266734080</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="7">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5">
         <v>16</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="19">
+      <c r="E8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="13">
         <f>F7/8</f>
-        <v>66683520</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>33341760</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="7">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5">
         <f>C7*C8</f>
         <v>166708800</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="22">
+      <c r="E9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="16">
         <f>F8/1024/1024</f>
-        <v>63.5943603515625</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+        <v>31.79718017578125</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="7">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
         <f>C9/8</f>
         <v>20838600</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="8">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6">
         <f>C10/1024/1024</f>
         <v>19.873237609863281</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="12">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="12">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="12">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8">
         <f>C15*C9</f>
         <v>666835200</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="12">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="8">
         <f>C16/8</f>
         <v>83354400</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="13">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9">
         <f>C17/1024/1024</f>
         <v>79.492950439453125</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="12">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="8">
         <v>2.5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="12">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="8">
         <f>C16/C19</f>
         <v>266734080</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="12">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="8">
         <f>C20/8</f>
         <v>33341760</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="15">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="11">
         <f>C21/1024/1024</f>
         <v>31.79718017578125</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First proposal for data transmitter and data receiver done
</commit_message>
<xml_diff>
--- a/FPGA_Developments/USB_3_FTDI/Documentation/Transfer Timing Analysis.xlsx
+++ b/FPGA_Developments/USB_3_FTDI/Documentation/Transfer Timing Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rfranca\Development\GitLab\simutemp\FPGA_Developments\USB_3_FTDI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rfranca\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37C4E55-4509-472A-ABA7-9BB2A4D737D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2829B8AF-607C-4C68-83E5-7C6B5CEA5AF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EE54F853-42C2-447C-92F1-1D14CFBF6EF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE54F853-42C2-447C-92F1-1D14CFBF6EF8}"/>
   </bookViews>
   <sheets>
     <sheet name="N-FEE" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+  <si>
+    <t>Rows (px)</t>
+  </si>
+  <si>
+    <t>Pixel (bits)</t>
+  </si>
+  <si>
+    <t>Overscan (px)</t>
+  </si>
   <si>
     <t>Total Pixels</t>
   </si>
   <si>
+    <t>Total Size (bits)</t>
+  </si>
+  <si>
+    <t>Total Size (Bytes)</t>
+  </si>
+  <si>
+    <t>E Columns (px)</t>
+  </si>
+  <si>
+    <t>F Columns (px)</t>
+  </si>
+  <si>
     <t>N-FEE caracteristics</t>
   </si>
   <si>
@@ -46,6 +67,27 @@
     <t>CCDs per camera</t>
   </si>
   <si>
+    <t>Readout Time (s)</t>
+  </si>
+  <si>
+    <t>Size per camera (bits)</t>
+  </si>
+  <si>
+    <t>Size per camera (Bytes)</t>
+  </si>
+  <si>
+    <t>Minimum data rate (bits/s)</t>
+  </si>
+  <si>
+    <t>Minimum data rate (Bytes/s)</t>
+  </si>
+  <si>
+    <t>Total Size (MBytes)</t>
+  </si>
+  <si>
+    <t>Minimum data rate (MBytes/s)</t>
+  </si>
+  <si>
     <t>F-FEE caracteristics</t>
   </si>
   <si>
@@ -58,6 +100,9 @@
     <t>Simulated cameras</t>
   </si>
   <si>
+    <t>Size per camera (MBytes)</t>
+  </si>
+  <si>
     <t>F-FEE CCD caracteristics</t>
   </si>
   <si>
@@ -85,6 +130,9 @@
     <t>Total Size [Bytes]</t>
   </si>
   <si>
+    <t>Total Size [Mbytes]</t>
+  </si>
+  <si>
     <t>Size per camera [bits]</t>
   </si>
   <si>
@@ -103,13 +151,10 @@
     <t>Minimum data rate [Bytes/s]</t>
   </si>
   <si>
+    <t>Minimum data rate [MBytes/s]</t>
+  </si>
+  <si>
     <t>Total Size [MBytes]</t>
-  </si>
-  <si>
-    <t>Minimum data rate [MiBytes/s]</t>
-  </si>
-  <si>
-    <t>Total Size [MiBytes]</t>
   </si>
 </sst>
 </file>
@@ -303,6 +348,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,6 +361,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -323,6 +380,12 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,24 +395,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,237 +713,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442A95F5-89D9-4832-937A-D9521D552F4E}">
   <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="E2" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
         <v>4510</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="E3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="19">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
         <v>30</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="19">
         <f>F3*C16</f>
         <v>10669363200</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
         <v>2295</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="E5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="19">
         <f>F4/8</f>
         <v>1333670400</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
         <v>2295</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="14">
+      <c r="E6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="20">
         <f>F5/1024/1024</f>
         <v>1271.88720703125</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7">
         <f>(C3+C4)*(C5+C6)</f>
         <v>20838600</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19">
         <f>F4/C19</f>
         <v>426774528</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
         <v>16</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="E8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="19">
         <f>F7/8</f>
         <v>53346816</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
         <f>C7*C8</f>
         <v>333417600</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="16">
+      <c r="E9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="22">
         <f>F8/1024/1024</f>
         <v>50.87548828125</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
         <f>C9/8</f>
         <v>41677200</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8">
         <f>C10/1024/1024</f>
         <v>39.746475219726563</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="12">
         <v>1</v>
       </c>
-      <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8">
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="8">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12">
         <f>C15*C9</f>
         <v>1333670400</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="8">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="12">
         <f>C16/8</f>
         <v>166708800</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="9">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="13">
         <f>C17/1024/1024</f>
         <v>158.98590087890625</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="8">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="8">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="12">
         <f>C16/C19</f>
         <v>53346816</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="8">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="12">
         <f>C20/8</f>
         <v>6668352</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="11">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="15">
         <f>C21/1024/1024</f>
         <v>6.35943603515625</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
     </row>
   </sheetData>
@@ -916,239 +959,239 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDD0D2E-3209-4761-BD12-93CDA5EAFBEA}">
   <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="E2" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6">
         <f>4510/2</f>
         <v>2255</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5">
+        <v>26</v>
+      </c>
+      <c r="C4" s="7">
         <f>30/2</f>
         <v>15</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="19">
         <f>F3*C16</f>
-        <v>666835200</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1333670400</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7">
         <v>2295</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="E5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="19">
         <f>F4/8</f>
-        <v>83354400</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>166708800</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7">
         <v>2295</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="14">
+      <c r="E6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="20">
         <f>F5/1024/1024</f>
-        <v>79.492950439453125</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>158.98590087890625</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7">
         <f>(C3+C4)*(C5+C6)</f>
         <v>10419300</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="19">
         <f>F4/C19</f>
-        <v>266734080</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>533468160</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5">
+        <v>29</v>
+      </c>
+      <c r="C8" s="7">
         <v>16</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="E8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="19">
         <f>F7/8</f>
-        <v>33341760</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66683520</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7">
         <f>C7*C8</f>
         <v>166708800</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="16">
+      <c r="E9" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="22">
         <f>F8/1024/1024</f>
-        <v>31.79718017578125</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63.5943603515625</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7">
         <f>C9/8</f>
         <v>20838600</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8">
         <f>C10/1024/1024</f>
         <v>19.873237609863281</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="12">
         <v>4</v>
       </c>
-      <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="8">
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="12">
         <f>C15*C9</f>
         <v>666835200</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="8">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="12">
         <f>C16/8</f>
         <v>83354400</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="9">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="13">
         <f>C17/1024/1024</f>
         <v>79.492950439453125</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="8">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="8">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="12">
         <f>C16/C19</f>
         <v>266734080</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="8">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="12">
         <f>C20/8</f>
         <v>33341760</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="11">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="15">
         <f>C21/1024/1024</f>
         <v>31.79718017578125</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
     </row>
   </sheetData>

</xml_diff>